<commit_message>
add new results to MAP
</commit_message>
<xml_diff>
--- a/excel/MAP.xlsx
+++ b/excel/MAP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OU\master\rm\pre_shot_sniper_detection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OU\master\rm\pre_shot_sniper_detection\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DBBCB7-E942-4A99-AD87-4CEE62F1CC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A745A0-C8BE-49BE-8B88-6B6986497CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39570" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7830" yWindow="5085" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="augmented_normal" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t># imgs</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>mAP50-95 val</t>
+  </si>
+  <si>
+    <t>augmentation</t>
   </si>
 </sst>
 </file>
@@ -383,12 +386,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC623A6-B8AA-416F-89D2-4720A6E7813D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>350</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>0.70035297086829296</v>
+      </c>
+      <c r="D2">
+        <v>0.29831424425049102</v>
+      </c>
+      <c r="E2">
+        <v>0.69996472803546395</v>
+      </c>
+      <c r="F2">
+        <v>0.29838620068163502</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>350</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>0.78923872125068495</v>
+      </c>
+      <c r="D3">
+        <v>0.31617320922684</v>
+      </c>
+      <c r="E3">
+        <v>0.78929014193262603</v>
+      </c>
+      <c r="F3">
+        <v>0.31612969102160698</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>350</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+      <c r="C4">
+        <v>0.83084999237384405</v>
+      </c>
+      <c r="D4">
+        <v>0.42006941518102597</v>
+      </c>
+      <c r="E4">
+        <v>0.82940956337066996</v>
+      </c>
+      <c r="F4">
+        <v>0.419667219059496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>350</v>
+      </c>
+      <c r="B5">
+        <v>0.4</v>
+      </c>
+      <c r="C5">
+        <v>0.87583359313041798</v>
+      </c>
+      <c r="D5">
+        <v>0.42719661182555801</v>
+      </c>
+      <c r="E5">
+        <v>0.87602208880721399</v>
+      </c>
+      <c r="F5">
+        <v>0.42343376030268098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>350</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>0.95690476190476104</v>
+      </c>
+      <c r="D6">
+        <v>0.57743818197682495</v>
+      </c>
+      <c r="E6">
+        <v>0.95690476190476104</v>
+      </c>
+      <c r="F6">
+        <v>0.57743998049110601</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -398,7 +531,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add sample data in csv
</commit_message>
<xml_diff>
--- a/excel/MAP.xlsx
+++ b/excel/MAP.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OU\master\rm\pre_shot_sniper_detection\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A745A0-C8BE-49BE-8B88-6B6986497CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3289886D-FAF0-4C94-A116-7A9827AB1ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7830" yWindow="5085" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38835" yWindow="705" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="augmented_normal" sheetId="3" r:id="rId1"/>
-    <sheet name="normal" sheetId="2" r:id="rId2"/>
-    <sheet name="small" sheetId="1" r:id="rId3"/>
+    <sheet name="background" sheetId="4" r:id="rId1"/>
+    <sheet name="augmented_normal" sheetId="3" r:id="rId2"/>
+    <sheet name="normal" sheetId="2" r:id="rId3"/>
+    <sheet name="small" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
-  <si>
-    <t># imgs</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>mAP50 train</t>
   </si>
@@ -45,13 +43,46 @@
   </si>
   <si>
     <t>augmentation</t>
+  </si>
+  <si>
+    <t># images</t>
+  </si>
+  <si>
+    <t># Images</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>mAP50</t>
+  </si>
+  <si>
+    <t>mAP50-95</t>
+  </si>
+  <si>
+    <t>fitness</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>dessert</t>
+  </si>
+  <si>
+    <t>rural</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +111,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -101,11 +137,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,14 +427,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693C4FE2-48CE-4846-ADD9-1B42A355B84E}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.78040800208070005</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.56603773584905603</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.60745433046712105</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.33173847281368102</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.35931005857902498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.75952319037496496</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.56603773584905603</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.56350751522794595</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.30575799343264698</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.331532945612177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.67</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC623A6-B8AA-416F-89D2-4720A6E7813D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
@@ -401,123 +547,123 @@
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>350</v>
       </c>
       <c r="B2">
         <v>0.1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>0.70035297086829296</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>0.29831424425049102</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>0.69996472803546395</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>0.29838620068163502</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>350</v>
       </c>
       <c r="B3">
         <v>0.2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>0.78923872125068495</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>0.31617320922684</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>0.78929014193262603</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>0.31612969102160698</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>350</v>
       </c>
       <c r="B4">
         <v>0.3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>0.83084999237384405</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>0.42006941518102597</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>0.82940956337066996</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>0.419667219059496</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>350</v>
       </c>
       <c r="B5">
         <v>0.4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>0.87583359313041798</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>0.42719661182555801</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>0.87602208880721399</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>0.42343376030268098</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>350</v>
       </c>
       <c r="B6">
         <v>0.5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>0.95690476190476104</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>0.57743818197682495</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>0.95690476190476104</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>0.57743998049110601</v>
       </c>
     </row>
@@ -526,15 +672,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E68BB5-4E41-49EF-BEFE-76394971BD72}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
@@ -542,207 +688,207 @@
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>100</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>0.504</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>0.17199999999999999</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>0.504</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>150</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>0.74099999999999999</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>0.496</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>0.74199999999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>0.496</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>200</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>0.77700000000000002</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>0.53400000000000003</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>0.77800000000000002</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>250</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>0.81299999999999994</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>0.81299999999999994</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>0.55700000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>300</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>0.746</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>0.54400000000000004</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>0.745</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>0.54300000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="3" customFormat="1">
       <c r="A7" s="3">
         <v>350</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="6">
         <v>0.88700000000000001</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>0.621</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>0.88700000000000001</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>0.61899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>400</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>0.88400000000000001</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>0.66400000000000003</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>0.88400000000000001</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>0.64400000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>450</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>0.85399999999999998</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>0.58799999999999997</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>0.85399999999999998</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>0.58899999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>500</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>0.84799999999999998</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>0.59399999999999997</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>0.84799999999999998</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>0.59199999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>550</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>0.84899999999999998</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>0.61599999999999999</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>0.84699999999999998</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>0.61599999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>600</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>0.88800000000000001</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>0.63700000000000001</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>0.88700000000000001</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>0.63600000000000001</v>
       </c>
     </row>
@@ -751,15 +897,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
@@ -767,171 +913,161 @@
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>100</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>0.73499999999999999</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>0.47</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>0.73399999999999999</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>0.47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>150</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>0.73499999999999999</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>0.47</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>0.73399999999999999</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>0.47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>200</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>0.78700000000000003</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>0.51400000000000001</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>0.78700000000000003</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>0.51400000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>250</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>0.79100000000000004</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>0.50800000000000001</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>0.79100000000000004</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>300</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>0.70499999999999996</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>0.503</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>0.70499999999999996</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>0.503</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>350</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>0.85899999999999999</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>0.61899999999999999</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>0.85899999999999999</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>0.61699999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>400</v>
-      </c>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>450</v>
-      </c>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>500</v>
-      </c>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>550</v>
-      </c>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>600</v>
-      </c>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:6">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>

</xml_diff>